<commit_message>
Actualizar carga de archivo de unidades, plantilla, y insert que contemple fechas de inicio y fin
</commit_message>
<xml_diff>
--- a/uploads/educativa/Plantilla_cargarunidadeducativa.xlsx
+++ b/uploads/educativa/Plantilla_cargarunidadeducativa.xlsx
@@ -1,40 +1,89 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Antonio\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UTEG\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8E985AFE-7EC9-43D9-866B-97B9E7E84E94}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F144F80B-5EBE-4B51-BE4F-47D5E4ECDAFE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{F55572E9-A1E3-4617-B10C-00E04965C630}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{F55572E9-A1E3-4617-B10C-00E04965C630}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>UTEG</author>
+  </authors>
+  <commentList>
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{DBCB1CCC-8850-4307-A342-A1AA83958700}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>UTEG:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Formato ==&gt; YYYY-MM-DD</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{88549AB7-1664-4CD6-948F-89BA571721D1}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>UTEG:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Formato ==&gt; YYYY-MM-DD</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Codigo Curso</t>
   </si>
@@ -44,12 +93,18 @@
   <si>
     <t>Nombre Unidad</t>
   </si>
+  <si>
+    <t>fecha_inicio</t>
+  </si>
+  <si>
+    <t>fecha_fin</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -64,6 +119,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -86,9 +154,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -402,21 +472,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81833F61-5BE7-48EA-8F0F-576982E4C744}">
-  <dimension ref="A1:C1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81833F61-5BE7-48EA-8F0F-576982E4C744}">
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.77734375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="11.5546875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -426,9 +497,16 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>